<commit_message>
Committing SBT First Code
</commit_message>
<xml_diff>
--- a/data/excel/modify.xlsx
+++ b/data/excel/modify.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\projectQuadlabs\data\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D2846E-E2CD-44BD-9830-2CCDA1E075E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14625" windowHeight="6705"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mfytest" sheetId="2" r:id="rId1"/>
     <sheet name="Duration" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="L1:Y20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,10 +523,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -713,7 +718,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -721,14 +726,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -806,7 +830,7 @@
         <v>48</v>
       </c>
       <c r="H2">
-        <v>2252020</v>
+        <v>8182022</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>37</v>
@@ -838,7 +862,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>